<commit_message>
v1.1 - new networks, config, disabling some functions
Added
-zkSync and linea networks
-beginnings of config system
--beginnings of networks enabling/disabling system
-plans md file
-time logs

Changed
-disabled all usdt/usdc functions (commented them for now)
</commit_message>
<xml_diff>
--- a/ethereum_balances.xlsx
+++ b/ethereum_balances.xlsx
@@ -446,22 +446,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>USDT</t>
+          <t>ETH_arb</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>ETH_linea</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>ETH_arb</t>
+          <t>ETH_op</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>USDT_arb</t>
+          <t>ETH_zksync</t>
         </is>
       </c>
     </row>
@@ -476,20 +476,22 @@
           <t>0.000084670896282</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.001536974079181586</t>
+        </is>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.001536974079181586</t>
+          <t>0.002200836190495412</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015099496454615183</t>
         </is>
       </c>
     </row>
@@ -504,20 +506,22 @@
           <t>0.008285731309625053</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>0</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.006650733812199677</t>
+        </is>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.006650733812199677</t>
+          <t>0.00521524178559823</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015176544130623508</t>
         </is>
       </c>
     </row>
@@ -532,20 +536,22 @@
           <t>0.008606634504338726</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.000895846210723599</t>
+        </is>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.000895846210723599</t>
+          <t>0.002135100732171918</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015176489122341696</t>
         </is>
       </c>
     </row>
@@ -560,20 +566,22 @@
           <t>0.008792175325772205</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.000991237831616832</t>
+        </is>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.000991237831616832</t>
+          <t>0.001624884842310747</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015172670325214127</t>
         </is>
       </c>
     </row>
@@ -588,20 +596,22 @@
           <t>0.008814428881570944</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.000849148022276697</t>
+        </is>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.000849148022276697</t>
+          <t>0.001895215160174945</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015125857492476492</t>
         </is>
       </c>
     </row>
@@ -616,20 +626,22 @@
           <t>0.004466408902601154</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>0</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.001649021765138309</t>
+        </is>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.001649021765138309</t>
+          <t>0.001488370167283218</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015149127631979354</t>
         </is>
       </c>
     </row>
@@ -644,20 +656,22 @@
           <t>0.00542886559896057</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>0</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.001605720112070093</t>
+        </is>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.001605720112070093</t>
+          <t>0.002053013326231324</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015116798681313845</t>
         </is>
       </c>
     </row>
@@ -672,20 +686,22 @@
           <t>0.004246914716146238</t>
         </is>
       </c>
-      <c r="C9" t="n">
-        <v>0</v>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.001115104203091896</t>
+        </is>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.001115104203091896</t>
+          <t>0.001983289096465981</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015198702062870001</t>
         </is>
       </c>
     </row>
@@ -700,20 +716,22 @@
           <t>0.003804951750408156</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>0</v>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.000812198319368855</t>
+        </is>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.000812198319368855</t>
+          <t>0.001663123103873953</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015255375021637252</t>
         </is>
       </c>
     </row>
@@ -728,20 +746,22 @@
           <t>0.006807906134535149</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>0</v>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.002577627061192211</t>
+        </is>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.002577627061192211</t>
+          <t>0.001483688916342881</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015172954782635143</t>
         </is>
       </c>
     </row>
@@ -756,20 +776,22 @@
           <t>0.006639737978102047</t>
         </is>
       </c>
-      <c r="C12" t="n">
-        <v>0</v>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.000929553715031862</t>
+        </is>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.000929553715031862</t>
+          <t>0.001652235479665607</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015180848922078652</t>
         </is>
       </c>
     </row>
@@ -784,20 +806,22 @@
           <t>0.007063979752412768</t>
         </is>
       </c>
-      <c r="C13" t="n">
-        <v>0</v>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.002026776174081591</t>
+        </is>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0.002026776174081591</t>
+          <t>0.002137748200075364</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015160322659445499</t>
         </is>
       </c>
     </row>
@@ -812,20 +836,22 @@
           <t>0.00656134474372661</t>
         </is>
       </c>
-      <c r="C14" t="n">
-        <v>0</v>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0.001512557278909545</t>
+        </is>
       </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0.001512557278909545</t>
+          <t>0.001958175685403652</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015103316942946463</t>
         </is>
       </c>
     </row>
@@ -840,20 +866,22 @@
           <t>0.007216516053446337</t>
         </is>
       </c>
-      <c r="C15" t="n">
-        <v>0</v>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0.001540379558857104</t>
+        </is>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0.001540379558857104</t>
+          <t>0.001296491744178415</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.016433254939550414</t>
         </is>
       </c>
     </row>
@@ -868,20 +896,22 @@
           <t>0.006611555606116423</t>
         </is>
       </c>
-      <c r="C16" t="n">
-        <v>0</v>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0.002869655016313948</t>
+        </is>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0.002869655016313948</t>
+          <t>0.005556224387734968</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015142242722078457</t>
         </is>
       </c>
     </row>
@@ -896,20 +926,22 @@
           <t>0.007108111865080358</t>
         </is>
       </c>
-      <c r="C17" t="n">
-        <v>0</v>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0.021865083811324299</t>
+        </is>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.021865083811324299</t>
+          <t>0.006771998882783559</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015193494536207619</t>
         </is>
       </c>
     </row>
@@ -924,20 +956,22 @@
           <t>0.005968375136393917</t>
         </is>
       </c>
-      <c r="C18" t="n">
-        <v>0</v>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0.00086302739174425</t>
+        </is>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.00086302739174425</t>
+          <t>0.00267645163747792</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015128569538923159</t>
         </is>
       </c>
     </row>
@@ -952,20 +986,22 @@
           <t>0.00608407661255332</t>
         </is>
       </c>
-      <c r="C19" t="n">
-        <v>0</v>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0.001990568969139395</t>
+        </is>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.001990568969139395</t>
+          <t>0.001864491364989403</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015124818183854209</t>
         </is>
       </c>
     </row>
@@ -980,20 +1016,22 @@
           <t>0.006526877660375492</t>
         </is>
       </c>
-      <c r="C20" t="n">
-        <v>0</v>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0.000844084533747813</t>
+        </is>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.000844084533747813</t>
+          <t>0.001985119617351436</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015184096214549963</t>
         </is>
       </c>
     </row>
@@ -1008,20 +1046,22 @@
           <t>0.005967189589539223</t>
         </is>
       </c>
-      <c r="C21" t="n">
-        <v>0</v>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0.001465992053809072</t>
+        </is>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0.001465992053809072</t>
+          <t>0.001932794729509414</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015185012825205172</t>
         </is>
       </c>
     </row>
@@ -1036,20 +1076,22 @@
           <t>0.005747434960620932</t>
         </is>
       </c>
-      <c r="C22" t="n">
-        <v>0</v>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0.001468279603900393</t>
+        </is>
       </c>
       <c r="D22" t="n">
         <v>0</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0.001468279603900393</t>
+          <t>0.001534215401876905</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015137931358804504</t>
         </is>
       </c>
     </row>
@@ -1064,20 +1106,22 @@
           <t>0.005999291259811385</t>
         </is>
       </c>
-      <c r="C23" t="n">
-        <v>0</v>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0.002378956371066653</t>
+        </is>
       </c>
       <c r="D23" t="n">
         <v>0</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.002378956371066653</t>
+          <t>0.006988865718991985</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015097292909320977</t>
         </is>
       </c>
     </row>
@@ -1092,20 +1136,22 @@
           <t>0.005755310702797986</t>
         </is>
       </c>
-      <c r="C24" t="n">
-        <v>0</v>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0.001196749928516341</t>
+        </is>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0.001196749928516341</t>
+          <t>0.006965630793153929</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015081014434191612</t>
         </is>
       </c>
     </row>
@@ -1120,20 +1166,22 @@
           <t>0.005657857909992558</t>
         </is>
       </c>
-      <c r="C25" t="n">
-        <v>0</v>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>0.00346368408562844</t>
+        </is>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0.00346368408562844</t>
+          <t>0.006946357939342155</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015146750449299984</t>
         </is>
       </c>
     </row>
@@ -1148,20 +1196,22 @@
           <t>0.005949703130852587</t>
         </is>
       </c>
-      <c r="C26" t="n">
-        <v>0</v>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0.000948170132526546</t>
+        </is>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>0.000948170132526546</t>
+          <t>0.001585244504725384</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015061511737303648</t>
         </is>
       </c>
     </row>
@@ -1176,20 +1226,22 @@
           <t>0.016471103996553953</t>
         </is>
       </c>
-      <c r="C27" t="n">
-        <v>0</v>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0.000833314387449408</t>
+        </is>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>0.000833314387449408</t>
+          <t>0.006976246037370431</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015128902268251703</t>
         </is>
       </c>
     </row>
@@ -1204,20 +1256,22 @@
           <t>0.006831602842873214</t>
         </is>
       </c>
-      <c r="C28" t="n">
-        <v>0</v>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>0.022407001336551327</t>
+        </is>
       </c>
       <c r="D28" t="n">
         <v>0</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0.022407001336551327</t>
+          <t>0.028968675830108055</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015085647067183624</t>
         </is>
       </c>
     </row>
@@ -1232,20 +1286,22 @@
           <t>0.006230016234684244</t>
         </is>
       </c>
-      <c r="C29" t="n">
-        <v>0</v>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>0.018480737235801809</t>
+        </is>
       </c>
       <c r="D29" t="n">
         <v>0</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0.018480737235801809</t>
+          <t>0.005367869708379562</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015281110689133648</t>
         </is>
       </c>
     </row>
@@ -1260,20 +1316,22 @@
           <t>0.006764248945757507</t>
         </is>
       </c>
-      <c r="C30" t="n">
-        <v>0</v>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>0.019188146201654576</t>
+        </is>
       </c>
       <c r="D30" t="n">
         <v>0</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0.019188146201654576</t>
+          <t>0.001755738659213979</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015189404034243648</t>
         </is>
       </c>
     </row>
@@ -1288,20 +1346,22 @@
           <t>0.001752498842794298</t>
         </is>
       </c>
-      <c r="C31" t="n">
-        <v>0</v>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0.001001021348714839</t>
+        </is>
       </c>
       <c r="D31" t="n">
         <v>0</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>0.001001021348714839</t>
+          <t>0.006896193222684303</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015090874380522679</t>
         </is>
       </c>
     </row>
@@ -1316,20 +1376,22 @@
           <t>0.002214431940211984</t>
         </is>
       </c>
-      <c r="C32" t="n">
-        <v>0</v>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>0.002482164796159314</t>
+        </is>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>0.002482164796159314</t>
+          <t>0.006535266711161772</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015070396443533648</t>
         </is>
       </c>
     </row>
@@ -1344,20 +1406,22 @@
           <t>0.00194924986711721</t>
         </is>
       </c>
-      <c r="C33" t="n">
-        <v>0</v>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0.001996061627776922</t>
+        </is>
       </c>
       <c r="D33" t="n">
         <v>0</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>0.001996061627776922</t>
+          <t>0.006155333459011032</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015213845002851701</t>
         </is>
       </c>
     </row>
@@ -1372,20 +1436,22 @@
           <t>0.002019316705485202</t>
         </is>
       </c>
-      <c r="C34" t="n">
-        <v>0</v>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>0.001118276434824176</t>
+        </is>
       </c>
       <c r="D34" t="n">
         <v>0</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0.001118276434824176</t>
+          <t>0.006906871344373532</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.01511098021385267</t>
         </is>
       </c>
     </row>
@@ -1400,20 +1466,22 @@
           <t>0.010329192837031268</t>
         </is>
       </c>
-      <c r="C35" t="n">
-        <v>0</v>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>0.001526387960676197</t>
+        </is>
       </c>
       <c r="D35" t="n">
         <v>0</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.001526387960676197</t>
+          <t>0.001514007941568989</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.01504176328428265</t>
         </is>
       </c>
     </row>
@@ -1428,20 +1496,22 @@
           <t>0.010081696169910332</t>
         </is>
       </c>
-      <c r="C36" t="n">
-        <v>0</v>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0.001513942906992883</t>
+        </is>
       </c>
       <c r="D36" t="n">
         <v>0</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0.001513942906992883</t>
+          <t>0.001545083728792859</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.0151344382245207</t>
         </is>
       </c>
     </row>
@@ -1456,20 +1526,22 @@
           <t>0.010239208435653416</t>
         </is>
       </c>
-      <c r="C37" t="n">
-        <v>0</v>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0.002481397792702547</t>
+        </is>
       </c>
       <c r="D37" t="n">
         <v>0</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0.002481397792702547</t>
+          <t>0.001326864850068064</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.01514273026063265</t>
         </is>
       </c>
     </row>
@@ -1484,20 +1556,22 @@
           <t>0.00344205341619952</t>
         </is>
       </c>
-      <c r="C38" t="n">
-        <v>0</v>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0.00321245559548818</t>
+        </is>
       </c>
       <c r="D38" t="n">
         <v>0</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>0.00321245559548818</t>
+          <t>0.001725108721096234</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.016338787896783631</t>
         </is>
       </c>
     </row>
@@ -1512,20 +1586,22 @@
           <t>0.00760297627242474</t>
         </is>
       </c>
-      <c r="C39" t="n">
-        <v>0</v>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0.00322099163141768</t>
+        </is>
       </c>
       <c r="D39" t="n">
         <v>0</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>0.00322099163141768</t>
+          <t>0.001695754682153717</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015148099980023624</t>
         </is>
       </c>
     </row>
@@ -1540,20 +1616,22 @@
           <t>0.009574627490483017</t>
         </is>
       </c>
-      <c r="C40" t="n">
-        <v>0</v>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0.003237695614920707</t>
+        </is>
       </c>
       <c r="D40" t="n">
         <v>0</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>0.003237695614920707</t>
+          <t>0.001728408079407527</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015086441825633624</t>
         </is>
       </c>
     </row>
@@ -1568,20 +1646,22 @@
           <t>0.007597669065527929</t>
         </is>
       </c>
-      <c r="C41" t="n">
-        <v>0</v>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0.003134053759281781</t>
+        </is>
       </c>
       <c r="D41" t="n">
         <v>0</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>0.003134053759281781</t>
+          <t>0.001685733263214249</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015110808620653624</t>
         </is>
       </c>
     </row>
@@ -1596,20 +1676,22 @@
           <t>0.041644632780462228</t>
         </is>
       </c>
-      <c r="C42" t="n">
-        <v>0</v>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0.001239517023106011</t>
+        </is>
       </c>
       <c r="D42" t="n">
         <v>0</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>0.001239517023106011</t>
+          <t>0.000686693733995163</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.01515590125</t>
         </is>
       </c>
     </row>
@@ -1624,20 +1706,22 @@
           <t>0.010480991121695883</t>
         </is>
       </c>
-      <c r="C43" t="n">
-        <v>0</v>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>0.002188145823964888</t>
+        </is>
       </c>
       <c r="D43" t="n">
         <v>0</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>0.002188145823964888</t>
+          <t>0.001434460115268412</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015186650543741681</t>
         </is>
       </c>
     </row>
@@ -1652,20 +1736,22 @@
           <t>0.011085515429929577</t>
         </is>
       </c>
-      <c r="C44" t="n">
-        <v>0</v>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0.002136234731372601</t>
+        </is>
       </c>
       <c r="D44" t="n">
         <v>0</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>0.002136234731372601</t>
+          <t>0.001505239975768865</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015082961982542655</t>
         </is>
       </c>
     </row>
@@ -1680,20 +1766,22 @@
           <t>0.011715131240267589</t>
         </is>
       </c>
-      <c r="C45" t="n">
-        <v>0</v>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0.002123361525496361</t>
+        </is>
       </c>
       <c r="D45" t="n">
         <v>0</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0.002123361525496361</t>
+          <t>0.001396992005637018</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015184672914401679</t>
         </is>
       </c>
     </row>
@@ -1708,20 +1796,22 @@
           <t>0.009611916828311839</t>
         </is>
       </c>
-      <c r="C46" t="n">
-        <v>0</v>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0.000748118137673123</t>
+        </is>
       </c>
       <c r="D46" t="n">
         <v>0</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>0.000748118137673123</t>
+          <t>0.001365037272692224</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015179290907403624</t>
         </is>
       </c>
     </row>
@@ -1736,20 +1826,22 @@
           <t>0.009459101602139784</t>
         </is>
       </c>
-      <c r="C47" t="n">
-        <v>0</v>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>0.00211383610362752</t>
+        </is>
       </c>
       <c r="D47" t="n">
         <v>0</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>0.00211383610362752</t>
+          <t>0.001377075770320885</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015103386821299719</t>
         </is>
       </c>
     </row>
@@ -1764,20 +1856,22 @@
           <t>0.013799528830675927</t>
         </is>
       </c>
-      <c r="C48" t="n">
-        <v>0</v>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0.002109775495194747</t>
+        </is>
       </c>
       <c r="D48" t="n">
         <v>0</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>0.002109775495194747</t>
+          <t>0.001336206939379119</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015103875136222641</t>
         </is>
       </c>
     </row>
@@ -1792,20 +1886,22 @@
           <t>0.013796201415101479</t>
         </is>
       </c>
-      <c r="C49" t="n">
-        <v>0</v>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0.002138077998804915</t>
+        </is>
       </c>
       <c r="D49" t="n">
         <v>0</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>0.002138077998804915</t>
+          <t>0.001323234685152189</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015241652762603622</t>
         </is>
       </c>
     </row>
@@ -1820,20 +1916,22 @@
           <t>0.01362343695970498</t>
         </is>
       </c>
-      <c r="C50" t="n">
-        <v>0</v>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>0.002134413658703638</t>
+        </is>
       </c>
       <c r="D50" t="n">
         <v>0</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>0.002134413658703638</t>
+          <t>0.001444960922498667</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015231633624792641</t>
         </is>
       </c>
     </row>
@@ -1848,20 +1946,22 @@
           <t>0.013157751152915982</t>
         </is>
       </c>
-      <c r="C51" t="n">
-        <v>0</v>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0.002146054834287665</t>
+        </is>
       </c>
       <c r="D51" t="n">
         <v>0</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>0.002146054834287665</t>
+          <t>0.00131202094708996</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.0150901723359507</t>
         </is>
       </c>
     </row>
@@ -1876,20 +1976,24 @@
           <t>0.000519732194152055</t>
         </is>
       </c>
-      <c r="C52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D52" t="n">
-        <v>8</v>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>0.001065695481281088</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0.02846647051653649</t>
+        </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>0.001065695481281088</t>
+          <t>0.001473325559169078</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015165315698868709</t>
         </is>
       </c>
     </row>
@@ -1904,20 +2008,24 @@
           <t>0.00520470450587952</t>
         </is>
       </c>
-      <c r="C53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D53" t="n">
-        <v>0</v>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>0.002920892588095877</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>0.028425680214173871</t>
+        </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>0.002920892588095877</t>
+          <t>0.001352156970233569</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.01520021724430667</t>
         </is>
       </c>
     </row>
@@ -1932,20 +2040,24 @@
           <t>0.007433525302227723</t>
         </is>
       </c>
-      <c r="C54" t="n">
-        <v>0</v>
-      </c>
-      <c r="D54" t="n">
-        <v>0</v>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>0.001294165369995486</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>0.028237495696581474</t>
+        </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>0.001294165369995486</t>
+          <t>0.001080181904172627</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015130150280226875</t>
         </is>
       </c>
     </row>
@@ -1960,20 +2072,24 @@
           <t>0.008292133743589462</t>
         </is>
       </c>
-      <c r="C55" t="n">
-        <v>0</v>
-      </c>
-      <c r="D55" t="n">
-        <v>0</v>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>0.001781683788601206</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>0.028419199010261388</t>
+        </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>0.001781683788601206</t>
+          <t>0.00146239008298656</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015103229927422268</t>
         </is>
       </c>
     </row>
@@ -1988,20 +2104,24 @@
           <t>0.008340841176973325</t>
         </is>
       </c>
-      <c r="C56" t="n">
-        <v>0</v>
-      </c>
-      <c r="D56" t="n">
-        <v>0</v>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0.001010548942832308</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0.028261909648041693</t>
+        </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>0.001010548942832308</t>
+          <t>0.001274187714531556</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015234557284383141</t>
         </is>
       </c>
     </row>
@@ -2016,20 +2136,24 @@
           <t>0.008232580095206091</t>
         </is>
       </c>
-      <c r="C57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D57" t="n">
-        <v>0</v>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>0.002021197701024969</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0.028388327285206513</t>
+        </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>0.002021197701024969</t>
+          <t>0.001796139665146785</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015172247841539798</t>
         </is>
       </c>
     </row>
@@ -2044,20 +2168,24 @@
           <t>0.00830173759015299</t>
         </is>
       </c>
-      <c r="C58" t="n">
-        <v>0</v>
-      </c>
-      <c r="D58" t="n">
-        <v>0</v>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>0.002730777178693714</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>0.028450647802057852</t>
+        </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>0.002730777178693714</t>
+          <t>0.001273762886168379</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.01511744237770285</t>
         </is>
       </c>
     </row>
@@ -2072,20 +2200,24 @@
           <t>0.008349021680871204</t>
         </is>
       </c>
-      <c r="C59" t="n">
-        <v>0</v>
-      </c>
-      <c r="D59" t="n">
-        <v>0</v>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0.001810207530441912</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0.028126773102295135</t>
+        </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>0.001810207530441912</t>
+          <t>0.001708602401400727</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015180773999533216</t>
         </is>
       </c>
     </row>
@@ -2100,20 +2232,24 @@
           <t>0.008878943955530206</t>
         </is>
       </c>
-      <c r="C60" t="n">
-        <v>0</v>
-      </c>
-      <c r="D60" t="n">
-        <v>0</v>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0.002240826160511478</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0.028401624409163199</t>
+        </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>0.002240826160511478</t>
+          <t>0.001109036269904536</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015195073610463794</t>
         </is>
       </c>
     </row>
@@ -2128,20 +2264,24 @@
           <t>0.009175359343551927</t>
         </is>
       </c>
-      <c r="C61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D61" t="n">
-        <v>0</v>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0.001570547153055433</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0.028333888194507543</t>
+        </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>0.001570547153055433</t>
+          <t>0.001246554603928167</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015207498875896864</t>
         </is>
       </c>
     </row>
@@ -2156,20 +2296,24 @@
           <t>0.007686580151709695</t>
         </is>
       </c>
-      <c r="C62" t="n">
-        <v>0</v>
-      </c>
-      <c r="D62" t="n">
-        <v>0</v>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>0.002120392121041885</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>0.02814781025045381</t>
+        </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>0.002120392121041885</t>
+          <t>0.001259801193973763</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.000085661225003894</t>
         </is>
       </c>
     </row>
@@ -2184,20 +2328,24 @@
           <t>0.008371346907018283</t>
         </is>
       </c>
-      <c r="C63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D63" t="n">
-        <v>0</v>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>0.0018118515220194</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>0.028328089512886782</t>
+        </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>0.0018118515220194</t>
+          <t>0.001059335078061579</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015126611999426629</t>
         </is>
       </c>
     </row>
@@ -2212,20 +2360,24 @@
           <t>0.007887085134122647</t>
         </is>
       </c>
-      <c r="C64" t="n">
-        <v>0</v>
-      </c>
-      <c r="D64" t="n">
-        <v>0</v>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>0.001471583180264029</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>0.028093687292859665</t>
+        </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>0.001471583180264029</t>
+          <t>0.001332055232610982</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015147526015047197</t>
         </is>
       </c>
     </row>
@@ -2240,20 +2392,24 @@
           <t>0.008158376275672885</t>
         </is>
       </c>
-      <c r="C65" t="n">
-        <v>0</v>
-      </c>
-      <c r="D65" t="n">
-        <v>0</v>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>0.002022308233702117</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>0.02821669539371679</t>
+        </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>0.002022308233702117</t>
+          <t>0.00115281824477365</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015197011862548334</t>
         </is>
       </c>
     </row>
@@ -2268,20 +2424,24 @@
           <t>0.008008408232889652</t>
         </is>
       </c>
-      <c r="C66" t="n">
-        <v>0</v>
-      </c>
-      <c r="D66" t="n">
-        <v>0</v>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>0.002102094872039664</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>0.028147815413161124</t>
+        </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>0.002102094872039664</t>
+          <t>0.001285881855635335</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015217209738616216</t>
         </is>
       </c>
     </row>
@@ -2296,20 +2456,24 @@
           <t>0.000477072274772077</t>
         </is>
       </c>
-      <c r="C67" t="n">
-        <v>0</v>
-      </c>
-      <c r="D67" t="n">
-        <v>0</v>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>0.004219765961454299</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>0.028473859060892187</t>
+        </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>0.004219765961454299</t>
+          <t>0.001833304936282787</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015087071536103347</t>
         </is>
       </c>
     </row>
@@ -2324,20 +2488,24 @@
           <t>0.000172707935219024</t>
         </is>
       </c>
-      <c r="C68" t="n">
-        <v>0</v>
-      </c>
-      <c r="D68" t="n">
-        <v>0</v>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>0.003132428030008305</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>0.027325186303633706</t>
+        </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>0.003132428030008305</t>
+          <t>0.001255004833943484</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015204269453907454</t>
         </is>
       </c>
     </row>
@@ -2352,20 +2520,24 @@
           <t>0.000374121555189001</t>
         </is>
       </c>
-      <c r="C69" t="n">
-        <v>0</v>
-      </c>
-      <c r="D69" t="n">
-        <v>0</v>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0.002380365545883525</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0.032721856309667415</t>
+        </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>0.002380365545883525</t>
+          <t>0.001216295913372081</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015085888476090345</t>
         </is>
       </c>
     </row>
@@ -2380,20 +2552,24 @@
           <t>0.000148602464987065</t>
         </is>
       </c>
-      <c r="C70" t="n">
-        <v>0</v>
-      </c>
-      <c r="D70" t="n">
-        <v>0</v>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>0.001950915189423252</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>0.032168055438447103</t>
+        </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>0.001950915189423252</t>
+          <t>0.001933206533423739</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.0151597194417841</t>
         </is>
       </c>
     </row>
@@ -2408,20 +2584,24 @@
           <t>0.000356405003699447</t>
         </is>
       </c>
-      <c r="C71" t="n">
-        <v>0</v>
-      </c>
-      <c r="D71" t="n">
-        <v>0</v>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>0.001379763689141741</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>0.030261890882806431</t>
+        </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>0.001379763689141741</t>
+          <t>0.00182061041733268</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015179520508399497</t>
         </is>
       </c>
     </row>
@@ -2436,20 +2616,24 @@
           <t>0.000396708333764308</t>
         </is>
       </c>
-      <c r="C72" t="n">
-        <v>0</v>
-      </c>
-      <c r="D72" t="n">
-        <v>0</v>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>0.003121442256208156</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>0.028617022712428566</t>
+        </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>0.003121442256208156</t>
+          <t>0.001489613072390388</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015150373058915061</t>
         </is>
       </c>
     </row>
@@ -2464,20 +2648,24 @@
           <t>0.000497896703119707</t>
         </is>
       </c>
-      <c r="C73" t="n">
-        <v>0</v>
-      </c>
-      <c r="D73" t="n">
-        <v>0</v>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>0.001723973119926255</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>0.02952097033314789</t>
+        </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>0.001723973119926255</t>
+          <t>0.001511124285991686</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015190575781436488</t>
         </is>
       </c>
     </row>
@@ -2492,20 +2680,24 @@
           <t>0.000181437323231652</t>
         </is>
       </c>
-      <c r="C74" t="n">
-        <v>0</v>
-      </c>
-      <c r="D74" t="n">
-        <v>0</v>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>0.001011905169039887</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>0.02883347197225529</t>
+        </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>0.001011905169039887</t>
+          <t>0.001146886792482124</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015152643773083303</t>
         </is>
       </c>
     </row>
@@ -2520,20 +2712,24 @@
           <t>0.000417782654624754</t>
         </is>
       </c>
-      <c r="C75" t="n">
-        <v>0</v>
-      </c>
-      <c r="D75" t="n">
-        <v>0</v>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>0.001350565262983579</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>0.028542545315584325</t>
+        </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>0.001350565262983579</t>
+          <t>0.001138283043640316</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015174670423348568</t>
         </is>
       </c>
     </row>
@@ -2548,20 +2744,24 @@
           <t>0.000191072678986312</t>
         </is>
       </c>
-      <c r="C76" t="n">
-        <v>0</v>
-      </c>
-      <c r="D76" t="n">
-        <v>0</v>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>0.001010091930807021</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>0.027874395111667421</t>
+        </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>0.001010091930807021</t>
+          <t>0.001686374953623174</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015198119460064174</t>
         </is>
       </c>
     </row>
@@ -2576,20 +2776,24 @@
           <t>0.00020275260315446</t>
         </is>
       </c>
-      <c r="C77" t="n">
-        <v>0</v>
-      </c>
-      <c r="D77" t="n">
-        <v>0</v>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>0.001678395128431993</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>0.027960244500396393</t>
+        </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>0.001678395128431993</t>
+          <t>0.001090854388742621</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015127381205620652</t>
         </is>
       </c>
     </row>
@@ -2604,20 +2808,24 @@
           <t>0.0001384904139689</t>
         </is>
       </c>
-      <c r="C78" t="n">
-        <v>0</v>
-      </c>
-      <c r="D78" t="n">
-        <v>0</v>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>0.001229315033520189</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>0.028057593556592169</t>
+        </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>0.001229315033520189</t>
+          <t>0.001212317632533659</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015107748702400526</t>
         </is>
       </c>
     </row>
@@ -2632,20 +2840,24 @@
           <t>0.000478806796188927</t>
         </is>
       </c>
-      <c r="C79" t="n">
-        <v>0</v>
-      </c>
-      <c r="D79" t="n">
-        <v>0</v>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>0.00194914232439254</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>0.028474571932921808</t>
+        </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>0.00194914232439254</t>
+          <t>0.001227610490510062</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015192932611938536</t>
         </is>
       </c>
     </row>
@@ -2660,20 +2872,24 @@
           <t>0.000241198188930819</t>
         </is>
       </c>
-      <c r="C80" t="n">
-        <v>0</v>
-      </c>
-      <c r="D80" t="n">
-        <v>0</v>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>0.002468507709606188</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>0.02713182051301753</t>
+        </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>0.002468507709606188</t>
+          <t>0.001436726010288015</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015210373002408372</t>
         </is>
       </c>
     </row>
@@ -2688,20 +2904,24 @@
           <t>0.000226025729733157</t>
         </is>
       </c>
-      <c r="C81" t="n">
-        <v>0</v>
-      </c>
-      <c r="D81" t="n">
-        <v>0</v>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>0.002050398240245688</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>0.027365933878516829</t>
+        </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>0.002050398240245688</t>
+          <t>0.001027979331134178</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015219242318080282</t>
         </is>
       </c>
     </row>
@@ -2716,20 +2936,24 @@
           <t>0.000163333658920599</t>
         </is>
       </c>
-      <c r="C82" t="n">
-        <v>0</v>
-      </c>
-      <c r="D82" t="n">
-        <v>0</v>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>0.003464101571704912</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>0.027332330859437399</t>
+        </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>0.003464101571704912</t>
+          <t>0.001912749857251252</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015096423074437814</t>
         </is>
       </c>
     </row>
@@ -2744,20 +2968,24 @@
           <t>0.000333124308475531</t>
         </is>
       </c>
-      <c r="C83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D83" t="n">
-        <v>0</v>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>0.002298351140892121</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>0.02715017147482356</t>
+        </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>0.002298351140892121</t>
+          <t>0.001053473250602096</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015149234939587917</t>
         </is>
       </c>
     </row>
@@ -2772,20 +3000,24 @@
           <t>0.000728145610195215</t>
         </is>
       </c>
-      <c r="C84" t="n">
-        <v>0</v>
-      </c>
-      <c r="D84" t="n">
-        <v>0</v>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>0.001997704845003626</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>0.026942297626387895</t>
+        </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>0.001997704845003626</t>
+          <t>0.001325625319249775</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015131780477591974</t>
         </is>
       </c>
     </row>
@@ -2800,20 +3032,24 @@
           <t>0.00103425030192643</t>
         </is>
       </c>
-      <c r="C85" t="n">
-        <v>0</v>
-      </c>
-      <c r="D85" t="n">
-        <v>0</v>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>0.002477779184407636</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>0.028490045552660349</t>
+        </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>0.002477779184407636</t>
+          <t>0.001351362026756053</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015219009764980229</t>
         </is>
       </c>
     </row>
@@ -2828,20 +3064,24 @@
           <t>0.00205248065853965</t>
         </is>
       </c>
-      <c r="C86" t="n">
-        <v>0</v>
-      </c>
-      <c r="D86" t="n">
-        <v>0</v>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>0.001940489810322923</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>0.02942061163559607</t>
+        </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>0.001940489810322923</t>
+          <t>0.001073624958715281</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.0151152049716855</t>
         </is>
       </c>
     </row>
@@ -2856,20 +3096,24 @@
           <t>0.0024021711651418</t>
         </is>
       </c>
-      <c r="C87" t="n">
-        <v>0</v>
-      </c>
-      <c r="D87" t="n">
-        <v>0</v>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>0.001958102101488046</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>0.027487614117409531</t>
+        </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>0.001958102101488046</t>
+          <t>0.00103322510816264</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015195177693997175</t>
         </is>
       </c>
     </row>
@@ -2884,20 +3128,24 @@
           <t>0.003772248738006751</t>
         </is>
       </c>
-      <c r="C88" t="n">
-        <v>0</v>
-      </c>
-      <c r="D88" t="n">
-        <v>0</v>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>0.002255714582796508</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>0.028120142638262229</t>
+        </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>0.002255714582796508</t>
+          <t>0.001027417379635377</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015090989781468095</t>
         </is>
       </c>
     </row>
@@ -2912,20 +3160,24 @@
           <t>0.004439380287102796</t>
         </is>
       </c>
-      <c r="C89" t="n">
-        <v>0</v>
-      </c>
-      <c r="D89" t="n">
-        <v>0</v>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>0.002268988810511744</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>0.027724594735270515</t>
+        </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>0.002268988810511744</t>
+          <t>0.001049907140686047</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015198081567062105</t>
         </is>
       </c>
     </row>
@@ -2940,20 +3192,24 @@
           <t>0.000962295692962142</t>
         </is>
       </c>
-      <c r="C90" t="n">
-        <v>0</v>
-      </c>
-      <c r="D90" t="n">
-        <v>0</v>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>0.002035084643813745</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>0.028618121624058864</t>
+        </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>0.002035084643813745</t>
+          <t>0.001104711605733498</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015133512050852379</t>
         </is>
       </c>
     </row>
@@ -2968,20 +3224,24 @@
           <t>0.003210945535602665</t>
         </is>
       </c>
-      <c r="C91" t="n">
-        <v>0</v>
-      </c>
-      <c r="D91" t="n">
-        <v>0</v>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>0.003125705812081057</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>0.028488359043567372</t>
+        </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>0.003125705812081057</t>
+          <t>0.001722428409873749</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015212502995313673</t>
         </is>
       </c>
     </row>
@@ -2996,20 +3256,22 @@
           <t>0.002585909256784573</t>
         </is>
       </c>
-      <c r="C92" t="n">
-        <v>0</v>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>0.001801142001883399</t>
+        </is>
       </c>
       <c r="D92" t="n">
         <v>0</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>0.001801142001883399</t>
+          <t>0.001074563621035278</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015164729055557709</t>
         </is>
       </c>
     </row>
@@ -3024,20 +3286,24 @@
           <t>0.002901797456919635</t>
         </is>
       </c>
-      <c r="C93" t="n">
-        <v>0</v>
-      </c>
-      <c r="D93" t="n">
-        <v>0</v>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>0.00186137714202042</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>6.3E-14</t>
+        </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>0.00186137714202042</t>
+          <t>0.00104892441152464</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015209413303378703</t>
         </is>
       </c>
     </row>
@@ -3052,20 +3318,24 @@
           <t>0.001913991800369286</t>
         </is>
       </c>
-      <c r="C94" t="n">
-        <v>0</v>
-      </c>
-      <c r="D94" t="n">
-        <v>0</v>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>0.003742406575187048</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>0.000005111190961017</t>
+        </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>0.003742406575187048</t>
+          <t>0.001594045073531235</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015222546484549671</t>
         </is>
       </c>
     </row>
@@ -3080,20 +3350,24 @@
           <t>0.003087677678501798</t>
         </is>
       </c>
-      <c r="C95" t="n">
-        <v>0</v>
-      </c>
-      <c r="D95" t="n">
-        <v>0</v>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>0.002074288403248623</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>0.028528528278438175</t>
+        </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>0.002074288403248623</t>
+          <t>0.001479136022820603</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015137512455766257</t>
         </is>
       </c>
     </row>
@@ -3108,20 +3382,24 @@
           <t>0.00475576895993866</t>
         </is>
       </c>
-      <c r="C96" t="n">
-        <v>0</v>
-      </c>
-      <c r="D96" t="n">
-        <v>0</v>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>0.000729403039865997</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>0.02798139187608166</t>
+        </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>0.000729403039865997</t>
+          <t>0.000432361768235113</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015122223135242137</t>
         </is>
       </c>
     </row>
@@ -3136,20 +3414,24 @@
           <t>0.005192777206724865</t>
         </is>
       </c>
-      <c r="C97" t="n">
-        <v>0</v>
-      </c>
-      <c r="D97" t="n">
-        <v>0</v>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>0.001503438074349403</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>0.000004427723890012</t>
+        </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>0.001503438074349403</t>
+          <t>0.001768188802595249</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.01517650334745408</t>
         </is>
       </c>
     </row>
@@ -3164,20 +3446,24 @@
           <t>0.0039963540798152</t>
         </is>
       </c>
-      <c r="C98" t="n">
-        <v>0</v>
-      </c>
-      <c r="D98" t="n">
-        <v>0</v>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>0.00107149333944995</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>0.000019241062219013</t>
+        </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>0.00107149333944995</t>
+          <t>0.00119823435570017</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015217738936845375</t>
         </is>
       </c>
     </row>
@@ -3192,20 +3478,24 @@
           <t>0.007433219422877512</t>
         </is>
       </c>
-      <c r="C99" t="n">
-        <v>0</v>
-      </c>
-      <c r="D99" t="n">
-        <v>0</v>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>0.001648704246290515</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>0.000014949919542012</t>
+        </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>0.001648704246290515</t>
+          <t>0.001604026741577399</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015111291330032973</t>
         </is>
       </c>
     </row>
@@ -3220,20 +3510,24 @@
           <t>0.003354979523066932</t>
         </is>
       </c>
-      <c r="C100" t="n">
-        <v>0</v>
-      </c>
-      <c r="D100" t="n">
-        <v>0</v>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>0.001239440205840979</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>0.02770965844091444</t>
+        </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>0.001239440205840979</t>
+          <t>0.001229670788449995</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.015232834678531705</t>
         </is>
       </c>
     </row>
@@ -3248,20 +3542,24 @@
           <t>0.003356313556911932</t>
         </is>
       </c>
-      <c r="C101" t="n">
-        <v>0</v>
-      </c>
-      <c r="D101" t="n">
-        <v>0</v>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>0.000607318354271822</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>0.000005766893349011</t>
+        </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>0.000607318354271822</t>
+          <t>0.000269457736299954</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Ошибка при получении баланса USDT: ("The function 'balanceOf' was not found in this contract's abi.", ' Are you sure you provided the correct contract abi?')</t>
+          <t>0.0151891052910341</t>
         </is>
       </c>
     </row>

</xml_diff>